<commit_message>
Improve storage of assays.tsv
</commit_message>
<xml_diff>
--- a/examples/VLP-ELISA-submission-valid.xlsx
+++ b/examples/VLP-ELISA-submission-valid.xlsx
@@ -389,7 +389,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>- Antibody name: The antibody's CoVIC ID.</t>
+          <t>- Antibody label: The antibody's CoVIC ID.</t>
         </is>
       </c>
     </row>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Antibody name</t>
+          <t>Antibody label</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">

</xml_diff>